<commit_message>
flash cannon, metal claw
</commit_message>
<xml_diff>
--- a/resources/base/particle/_Moves.xlsx
+++ b/resources/base/particle/_Moves.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\projects\pokejets\ulix-dexflow\resources\base\particle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAB73D15-8933-4954-B7E6-858A18FD59D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A787F83-D259-4954-8B7A-E0682855C181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="672" windowWidth="22872" windowHeight="12216" activeTab="1" xr2:uid="{80E0F31D-A046-4CD3-826F-B4034176B7E3}"/>
+    <workbookView xWindow="60" yWindow="672" windowWidth="22872" windowHeight="12216" xr2:uid="{80E0F31D-A046-4CD3-826F-B4034176B7E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Attack move" sheetId="4" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2115" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="736">
   <si>
     <t>Sleep</t>
   </si>
@@ -2940,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB474F78-426D-432A-A4CC-F5C23881488B}">
   <dimension ref="A1:R677"/>
   <sheetViews>
-    <sheetView topLeftCell="A541" workbookViewId="0">
-      <selection activeCell="F553" sqref="F553"/>
+    <sheetView tabSelected="1" topLeftCell="A618" workbookViewId="0">
+      <selection activeCell="F628" sqref="F628"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="R9" s="27">
         <f>IF(Q9&lt;&gt;"",COUNTIF(F:F,Q9),"")</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -3808,11 +3808,11 @@
       </c>
       <c r="M25" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N25" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="Q25" s="22"/>
       <c r="R25" s="27" t="str">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="M29" s="24">
         <f>SUM(M9:M26)</f>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N29" s="25">
         <f>M29/L29</f>
-        <v>4.2899408284023666E-2</v>
+        <v>4.5857988165680472E-2</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -15921,8 +15921,8 @@
       <c r="E628" s="6" t="str">
         <v>Special</v>
       </c>
-      <c r="F628" s="6">
-        <v>0</v>
+      <c r="F628" s="6" t="str">
+        <v>Sipondo</v>
       </c>
     </row>
     <row r="629" spans="1:6" x14ac:dyDescent="0.3">
@@ -16081,8 +16081,8 @@
       <c r="E636" s="6" t="str">
         <v>Physical</v>
       </c>
-      <c r="F636" s="6">
-        <v>0</v>
+      <c r="F636" s="6" t="str">
+        <v>Sipondo</v>
       </c>
     </row>
     <row r="637" spans="1:6" x14ac:dyDescent="0.3">
@@ -16979,9 +16979,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A7B243-4A1E-44C3-B8AB-7381CB16F16D}">
   <dimension ref="A1:F677"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A545" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G553" sqref="G553"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A626" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I639" sqref="I639"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27681,7 +27681,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="625" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="625" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A625">
         <v>624</v>
       </c>
@@ -27698,7 +27698,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="626" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="626" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A626">
         <v>625</v>
       </c>
@@ -27715,7 +27715,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="627" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="627" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A627">
         <v>626</v>
       </c>
@@ -27732,7 +27732,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="628" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="628" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A628">
         <v>627</v>
       </c>
@@ -27748,8 +27748,11 @@
       <c r="E628" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="629" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F628" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="629" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A629">
         <v>628</v>
       </c>
@@ -27766,7 +27769,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="630" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="630" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A630">
         <v>629</v>
       </c>
@@ -27783,7 +27786,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="631" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="631" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A631">
         <v>630</v>
       </c>
@@ -27800,7 +27803,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="632" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="632" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A632">
         <v>631</v>
       </c>
@@ -27817,7 +27820,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="633" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="633" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A633">
         <v>632</v>
       </c>
@@ -27834,7 +27837,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="634" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="634" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A634">
         <v>633</v>
       </c>
@@ -27851,7 +27854,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="635" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="635" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A635">
         <v>634</v>
       </c>
@@ -27868,7 +27871,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="636" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="636" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A636">
         <v>635</v>
       </c>
@@ -27884,8 +27887,11 @@
       <c r="E636" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="637" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F636" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A637">
         <v>636</v>
       </c>
@@ -27902,7 +27908,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="638" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="638" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A638">
         <v>637</v>
       </c>
@@ -27919,7 +27925,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="639" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="639" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A639">
         <v>638</v>
       </c>
@@ -27936,7 +27942,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="640" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="640" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A640">
         <v>639</v>
       </c>

</xml_diff>

<commit_message>
aeroblast, gust, dragon pulse
</commit_message>
<xml_diff>
--- a/resources/base/particle/_Moves.xlsx
+++ b/resources/base/particle/_Moves.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\projects\pokejets\ulix-dexflow\resources\base\particle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A787F83-D259-4954-8B7A-E0682855C181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C54C945-116A-4E47-89C9-3035763A1AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="672" windowWidth="22872" windowHeight="12216" xr2:uid="{80E0F31D-A046-4CD3-826F-B4034176B7E3}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="736">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2122" uniqueCount="736">
   <si>
     <t>Sleep</t>
   </si>
@@ -2940,8 +2940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB474F78-426D-432A-A4CC-F5C23881488B}">
   <dimension ref="A1:R677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A618" workbookViewId="0">
-      <selection activeCell="F628" sqref="F628"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3173,7 +3173,7 @@
       </c>
       <c r="R9" s="27">
         <f>IF(Q9&lt;&gt;"",COUNTIF(F:F,Q9),"")</f>
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
@@ -3246,11 +3246,11 @@
       </c>
       <c r="M11" s="19">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N11" s="20">
         <f t="shared" si="0"/>
-        <v>6.25E-2</v>
+        <v>0.125</v>
       </c>
       <c r="Q11" s="22" t="str">
         <v>Piadith</v>
@@ -3328,11 +3328,11 @@
       </c>
       <c r="M13" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N13" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Q13" s="22"/>
       <c r="R13" s="27" t="str">
@@ -3448,11 +3448,11 @@
       </c>
       <c r="M16" s="19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="Q16" s="22"/>
       <c r="R16" s="27" t="str">
@@ -3938,11 +3938,11 @@
       </c>
       <c r="M29" s="24">
         <f>SUM(M9:M26)</f>
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="N29" s="25">
         <f>M29/L29</f>
-        <v>4.5857988165680472E-2</v>
+        <v>5.3254437869822487E-2</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -4841,8 +4841,8 @@
       <c r="E74" s="6" t="str">
         <v>Special</v>
       </c>
-      <c r="F74" s="6">
-        <v>0</v>
+      <c r="F74" s="6" t="str">
+        <v>Sipondo</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
@@ -5661,8 +5661,8 @@
       <c r="E115" s="6" t="str">
         <v>Special</v>
       </c>
-      <c r="F115" s="6">
-        <v>0</v>
+      <c r="F115" s="6" t="str">
+        <v>Sipondo</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.3">
@@ -5721,8 +5721,8 @@
       <c r="E118" s="6" t="str">
         <v>Special</v>
       </c>
-      <c r="F118" s="6">
-        <v>0</v>
+      <c r="F118" s="6" t="str">
+        <v>Sipondo</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.3">
@@ -7581,8 +7581,8 @@
       <c r="E211" s="6" t="str">
         <v>Special</v>
       </c>
-      <c r="F211" s="6">
-        <v>0</v>
+      <c r="F211" s="6" t="str">
+        <v>Sipondo</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.3">
@@ -7861,8 +7861,8 @@
       <c r="E225" s="6" t="str">
         <v>Special</v>
       </c>
-      <c r="F225" s="6">
-        <v>0</v>
+      <c r="F225" s="6" t="str">
+        <v>Sipondo</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">
@@ -16980,8 +16980,8 @@
   <dimension ref="A1:F677"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A626" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I639" sqref="I639"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18261,6 +18261,9 @@
       <c r="E74" t="s">
         <v>43</v>
       </c>
+      <c r="F74" t="s">
+        <v>729</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75">
@@ -18917,7 +18920,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>112</v>
       </c>
@@ -18934,7 +18937,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>113</v>
       </c>
@@ -18951,7 +18954,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>114</v>
       </c>
@@ -18967,8 +18970,11 @@
       <c r="E115" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F115" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>115</v>
       </c>
@@ -18985,7 +18991,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>116</v>
       </c>
@@ -19002,7 +19008,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>117</v>
       </c>
@@ -19018,8 +19024,11 @@
       <c r="E118" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F118" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>118</v>
       </c>
@@ -19036,7 +19045,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>119</v>
       </c>
@@ -19053,7 +19062,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>120</v>
       </c>
@@ -19070,7 +19079,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>121</v>
       </c>
@@ -19087,7 +19096,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>122</v>
       </c>
@@ -19104,7 +19113,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>123</v>
       </c>
@@ -19121,7 +19130,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>124</v>
       </c>
@@ -19138,7 +19147,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>125</v>
       </c>
@@ -19155,7 +19164,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>126</v>
       </c>
@@ -19172,7 +19181,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>127</v>
       </c>
@@ -20561,7 +20570,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>208</v>
       </c>
@@ -20578,7 +20587,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>209</v>
       </c>
@@ -20595,7 +20604,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>210</v>
       </c>
@@ -20611,8 +20620,11 @@
       <c r="E211" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F211" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>211</v>
       </c>
@@ -20629,7 +20641,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>212</v>
       </c>
@@ -20646,7 +20658,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>213</v>
       </c>
@@ -20663,7 +20675,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>214</v>
       </c>
@@ -20680,7 +20692,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>215</v>
       </c>
@@ -20697,7 +20709,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>216</v>
       </c>
@@ -20714,7 +20726,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>217</v>
       </c>
@@ -20731,7 +20743,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>218</v>
       </c>
@@ -20748,7 +20760,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>219</v>
       </c>
@@ -20765,7 +20777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>220</v>
       </c>
@@ -20782,7 +20794,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>221</v>
       </c>
@@ -20799,7 +20811,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>222</v>
       </c>
@@ -20816,7 +20828,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>223</v>
       </c>
@@ -20848,6 +20860,9 @@
       </c>
       <c r="E225" t="s">
         <v>43</v>
+      </c>
+      <c r="F225" t="s">
+        <v>729</v>
       </c>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>